<commit_message>
Adding new example and requirements
</commit_message>
<xml_diff>
--- a/Data/1-hour-interval-madrid/1-hour-interval-madrid/testsuite/results.xlsx
+++ b/Data/1-hour-interval-madrid/1-hour-interval-madrid/testsuite/results.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Model1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Model2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Model3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Model310" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -499,7 +499,7 @@
         <v>10771</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01400017738342285</v>
+        <v>0.0150001049041748</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
         <v>12304</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01699995994567871</v>
+        <v>0.01900005340576172</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -547,7 +547,7 @@
         <v>9519</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0130000114440918</v>
+        <v>0.01399993896484375</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -571,7 +571,7 @@
         <v>6897</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01200008392333984</v>
+        <v>0.01399993896484375</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
         <v>4998</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0130000114440918</v>
+        <v>0.01799988746643066</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -619,7 +619,7 @@
         <v>5913</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01399993896484375</v>
+        <v>0.01699995994567871</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
         <v>4135</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01199984550476074</v>
+        <v>0.01100015640258789</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -691,7 +691,7 @@
         <v>8576</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0130000114440918</v>
+        <v>0.01999998092651367</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -715,7 +715,7 @@
         <v>6139</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01199984550476074</v>
+        <v>0.0130000114440918</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -739,7 +739,7 @@
         <v>7277</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01399993896484375</v>
+        <v>0.01600003242492676</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -763,7 +763,7 @@
         <v>5314</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01399993896484375</v>
+        <v>0.0130000114440918</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         <v>7228</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0129997730255127</v>
+        <v>0.0130000114440918</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>8564</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0130000114440918</v>
+        <v>0.0149998664855957</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -835,7 +835,7 @@
         <v>8175</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01600003242492676</v>
+        <v>0.0130000114440918</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>5817</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01399993896484375</v>
+        <v>0.01699995994567871</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -883,7 +883,7 @@
         <v>4575</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0130000114440918</v>
+        <v>0.01200008392333984</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         <v>3852</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01200008392333984</v>
+        <v>0.01699995994567871</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -931,7 +931,7 @@
         <v>6506</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01400017738342285</v>
+        <v>0.01200008392333984</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -955,7 +955,7 @@
         <v>416</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01200008392333984</v>
+        <v>0.0130000114440918</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1030,7 +1030,7 @@
         <v>10771</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5740001201629639</v>
+        <v>0.4739999771118164</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1054,7 +1054,7 @@
         <v>12304</v>
       </c>
       <c r="D3" t="n">
-        <v>1.154999971389771</v>
+        <v>0.9619998931884766</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1078,7 +1078,7 @@
         <v>9519</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2689998149871826</v>
+        <v>0.2660000324249268</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -1102,7 +1102,7 @@
         <v>6599</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1099998950958252</v>
+        <v>0.1120002269744873</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1126,7 +1126,7 @@
         <v>4998</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0820000171661377</v>
+        <v>0.1119999885559082</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1150,7 +1150,7 @@
         <v>5721</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0840001106262207</v>
+        <v>0.1150000095367432</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>4135</v>
       </c>
       <c r="D8" t="n">
-        <v>0.07800006866455078</v>
+        <v>0.07299995422363281</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1198,7 +1198,7 @@
         <v>1602</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02999997138977051</v>
+        <v>0.03099989891052246</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
         <v>8576</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1230001449584961</v>
+        <v>0.1460001468658447</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1246,7 +1246,7 @@
         <v>6139</v>
       </c>
       <c r="D11" t="n">
-        <v>0.09400010108947754</v>
+        <v>0.1289999485015869</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1270,7 +1270,7 @@
         <v>7149</v>
       </c>
       <c r="D12" t="n">
-        <v>0.09999990463256836</v>
+        <v>0.1559998989105225</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1294,7 +1294,7 @@
         <v>5314</v>
       </c>
       <c r="D13" t="n">
-        <v>0.07299995422363281</v>
+        <v>0.1390001773834229</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
         <v>7109</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1579999923706055</v>
+        <v>0.18399977684021</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>8093</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1749999523162842</v>
+        <v>0.2349998950958252</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1366,7 +1366,7 @@
         <v>7541</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1009998321533203</v>
+        <v>0.1140000820159912</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
         <v>5817</v>
       </c>
       <c r="D17" t="n">
-        <v>0.09599995613098145</v>
+        <v>0.2019999027252197</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1414,7 +1414,7 @@
         <v>4575</v>
       </c>
       <c r="D18" t="n">
-        <v>0.07800006866455078</v>
+        <v>0.1150000095367432</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1438,7 +1438,7 @@
         <v>3615</v>
       </c>
       <c r="D19" t="n">
-        <v>0.09000015258789062</v>
+        <v>0.08299994468688965</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
         <v>6506</v>
       </c>
       <c r="D20" t="n">
-        <v>0.07999992370605469</v>
+        <v>0.1400001049041748</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>416</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01699995994567871</v>
+        <v>0.0280001163482666</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1563,13 +1563,13 @@
         <v>34</v>
       </c>
       <c r="C2" t="n">
-        <v>10778.99992640805</v>
+        <v>10770.99999469879</v>
       </c>
       <c r="D2" t="n">
-        <v>90.1010000705719</v>
+        <v>3600.618000030518</v>
       </c>
       <c r="E2" t="n">
-        <v>68</v>
+        <v>276</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>10926</v>
+        <v>227752</v>
       </c>
     </row>
     <row r="3">
@@ -1590,13 +1590,13 @@
         <v>36</v>
       </c>
       <c r="C3" t="n">
-        <v>12306.99987729298</v>
+        <v>12494.99997567427</v>
       </c>
       <c r="D3" t="n">
-        <v>90.08500003814697</v>
+        <v>3601.017999887466</v>
       </c>
       <c r="E3" t="n">
-        <v>72</v>
+        <v>308</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -1604,7 +1604,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>13245</v>
+        <v>279398</v>
       </c>
     </row>
     <row r="4">
@@ -1617,13 +1617,13 @@
         <v>32</v>
       </c>
       <c r="C4" t="n">
-        <v>9521.999966899311</v>
+        <v>9518.999783110961</v>
       </c>
       <c r="D4" t="n">
-        <v>90.07000017166138</v>
+        <v>3600.436000108719</v>
       </c>
       <c r="E4" t="n">
-        <v>64</v>
+        <v>258</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>10003</v>
+        <v>201072</v>
       </c>
     </row>
     <row r="5">
@@ -1644,13 +1644,13 @@
         <v>24</v>
       </c>
       <c r="C5" t="n">
-        <v>6598.999972250128</v>
+        <v>6598.999934106854</v>
       </c>
       <c r="D5" t="n">
-        <v>90.15999984741211</v>
+        <v>3600.695000171661</v>
       </c>
       <c r="E5" t="n">
-        <v>48</v>
+        <v>190</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -1658,7 +1658,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>5543</v>
+        <v>99268</v>
       </c>
     </row>
     <row r="6">
@@ -1671,21 +1671,21 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>4997.999963445223</v>
+        <v>4997.999683341697</v>
       </c>
       <c r="D6" t="n">
-        <v>3.393999814987183</v>
+        <v>3600.507999897003</v>
       </c>
       <c r="E6" t="n">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>3886</v>
+        <v>69916</v>
       </c>
     </row>
     <row r="7">
@@ -1698,21 +1698,21 @@
         <v>22</v>
       </c>
       <c r="C7" t="n">
-        <v>5720.999982279663</v>
+        <v>5720.999254496943</v>
       </c>
       <c r="D7" t="n">
-        <v>4.984999895095825</v>
+        <v>3600.757999897003</v>
       </c>
       <c r="E7" t="n">
-        <v>44</v>
+        <v>174</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>3889</v>
+        <v>79964</v>
       </c>
     </row>
     <row r="8">
@@ -1725,21 +1725,21 @@
         <v>20</v>
       </c>
       <c r="C8" t="n">
-        <v>4134.999933539038</v>
+        <v>4134.999177478211</v>
       </c>
       <c r="D8" t="n">
-        <v>1.475000143051147</v>
+        <v>3607.441999912262</v>
       </c>
       <c r="E8" t="n">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>3493</v>
+        <v>66950</v>
       </c>
     </row>
     <row r="9">
@@ -1752,13 +1752,13 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>1602</v>
+        <v>1601.999998358191</v>
       </c>
       <c r="D9" t="n">
-        <v>0.08599996566772461</v>
+        <v>0.8029999732971191</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1766,7 +1766,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>595</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="10">
@@ -1779,13 +1779,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="n">
-        <v>8575.999941942224</v>
+        <v>8575.999372841841</v>
       </c>
       <c r="D10" t="n">
-        <v>90.12600016593933</v>
+        <v>3600.623000144958</v>
       </c>
       <c r="E10" t="n">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1793,7 +1793,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>8569</v>
+        <v>176244</v>
       </c>
     </row>
     <row r="11">
@@ -1806,21 +1806,21 @@
         <v>26</v>
       </c>
       <c r="C11" t="n">
-        <v>6138.99997113376</v>
+        <v>6138.999382766653</v>
       </c>
       <c r="D11" t="n">
-        <v>6.233999967575073</v>
+        <v>3600.554000139236</v>
       </c>
       <c r="E11" t="n">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>6378</v>
+        <v>125484</v>
       </c>
     </row>
     <row r="12">
@@ -1833,13 +1833,13 @@
         <v>27</v>
       </c>
       <c r="C12" t="n">
-        <v>7148.999951728321</v>
+        <v>7148.999629195149</v>
       </c>
       <c r="D12" t="n">
-        <v>90.05599999427795</v>
+        <v>3600.576999902725</v>
       </c>
       <c r="E12" t="n">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1847,7 +1847,7 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>7039</v>
+        <v>135766</v>
       </c>
     </row>
     <row r="13">
@@ -1860,21 +1860,21 @@
         <v>24</v>
       </c>
       <c r="C13" t="n">
-        <v>5313.999952799319</v>
+        <v>5313.513460910006</v>
       </c>
       <c r="D13" t="n">
-        <v>12.18899989128113</v>
+        <v>3634.87700009346</v>
       </c>
       <c r="E13" t="n">
-        <v>48</v>
+        <v>192</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>5374</v>
+        <v>102906</v>
       </c>
     </row>
     <row r="14">
@@ -1887,21 +1887,21 @@
         <v>27</v>
       </c>
       <c r="C14" t="n">
-        <v>7108.999813137773</v>
+        <v>7108.998884280798</v>
       </c>
       <c r="D14" t="n">
-        <v>10.63299989700317</v>
+        <v>3600.973999977112</v>
       </c>
       <c r="E14" t="n">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>7129</v>
+        <v>141346</v>
       </c>
     </row>
     <row r="15">
@@ -1914,13 +1914,13 @@
         <v>29</v>
       </c>
       <c r="C15" t="n">
-        <v>8092.999962206151</v>
+        <v>8092.999516291501</v>
       </c>
       <c r="D15" t="n">
-        <v>90.05900001525879</v>
+        <v>3600.71799993515</v>
       </c>
       <c r="E15" t="n">
-        <v>58</v>
+        <v>240</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>8186</v>
+        <v>166110</v>
       </c>
     </row>
     <row r="16">
@@ -1941,13 +1941,13 @@
         <v>27</v>
       </c>
       <c r="C16" t="n">
-        <v>7540.999916911372</v>
+        <v>7540.621403651022</v>
       </c>
       <c r="D16" t="n">
-        <v>90.04699993133545</v>
+        <v>3600.673000097275</v>
       </c>
       <c r="E16" t="n">
-        <v>54</v>
+        <v>218</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1955,7 +1955,7 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>7245</v>
+        <v>135604</v>
       </c>
     </row>
     <row r="17">
@@ -1968,21 +1968,21 @@
         <v>24</v>
       </c>
       <c r="C17" t="n">
-        <v>5816.999928200907</v>
+        <v>5816.999102917282</v>
       </c>
       <c r="D17" t="n">
-        <v>4.301000118255615</v>
+        <v>3600.576999902725</v>
       </c>
       <c r="E17" t="n">
-        <v>48</v>
+        <v>192</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>5257</v>
+        <v>103886</v>
       </c>
     </row>
     <row r="18">
@@ -1995,21 +1995,21 @@
         <v>20</v>
       </c>
       <c r="C18" t="n">
-        <v>4574.999854645823</v>
+        <v>4574.998437223135</v>
       </c>
       <c r="D18" t="n">
-        <v>1.069999933242798</v>
+        <v>3600.417000055313</v>
       </c>
       <c r="E18" t="n">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>3493</v>
+        <v>66950</v>
       </c>
     </row>
     <row r="19">
@@ -2022,13 +2022,13 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>3614.999983532254</v>
+        <v>3615</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7669999599456787</v>
+        <v>2692.256999969482</v>
       </c>
       <c r="E19" t="n">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -2036,7 +2036,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>2753</v>
+        <v>44894</v>
       </c>
     </row>
     <row r="20">
@@ -2049,21 +2049,21 @@
         <v>26</v>
       </c>
       <c r="C20" t="n">
-        <v>6505.999982863876</v>
+        <v>6505.999870973515</v>
       </c>
       <c r="D20" t="n">
-        <v>3.936000108718872</v>
+        <v>3600.544999837875</v>
       </c>
       <c r="E20" t="n">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>optimal</t>
+          <t>maxTimeLimit</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>6883</v>
+        <v>142182</v>
       </c>
     </row>
     <row r="21">
@@ -2079,10 +2079,10 @@
         <v>416</v>
       </c>
       <c r="D21" t="n">
-        <v>0.07700014114379883</v>
+        <v>0.1380000114440918</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -2090,7 +2090,7 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>131</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>